<commit_message>
collected new literature and created bib file
</commit_message>
<xml_diff>
--- a/1_literature/literature-list.xlsx
+++ b/1_literature/literature-list.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5097F4A-667A-4647-A3C5-107A7B81BCAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42535091-B349-4DFF-B35F-6193E52D8908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>authors</t>
   </si>
@@ -103,6 +106,156 @@
   </si>
   <si>
     <t>original proposition of h-lle, contrast to laplacian and lle</t>
+  </si>
+  <si>
+    <t>tenenbaum, de silva, langford</t>
+  </si>
+  <si>
+    <t>a global geometric framework for nonlinear dimensionality reduction</t>
+  </si>
+  <si>
+    <t>isomap</t>
+  </si>
+  <si>
+    <t>original proposition of isomap</t>
+  </si>
+  <si>
+    <t>de silva, tenenbaum</t>
+  </si>
+  <si>
+    <t>global vs local methods in nonlinear dimensionality reduction</t>
+  </si>
+  <si>
+    <t>isomap, landmark isomap</t>
+  </si>
+  <si>
+    <t>global vs local, landmark algorithm</t>
+  </si>
+  <si>
+    <t>van der maaten, postma, van den herik</t>
+  </si>
+  <si>
+    <t>dimensionality reduction: a comparative review</t>
+  </si>
+  <si>
+    <t>review, meta analysis, dimensionality reduction</t>
+  </si>
+  <si>
+    <t>definition of dimensionality reduction</t>
+  </si>
+  <si>
+    <t>anderson, morley</t>
+  </si>
+  <si>
+    <t>eigenvalues of the laplacian of a graph</t>
+  </si>
+  <si>
+    <t>graph laplacian</t>
+  </si>
+  <si>
+    <t>probably original proposition</t>
+  </si>
+  <si>
+    <t>schwartz</t>
+  </si>
+  <si>
+    <t>the isomap algorithm and topological stability</t>
+  </si>
+  <si>
+    <t>perhaps for discussion</t>
+  </si>
+  <si>
+    <t>laplacian eigenmaps and spectral techniques for embedding and clustering</t>
+  </si>
+  <si>
+    <t>semi-supervised learning on riemannian manifolds</t>
+  </si>
+  <si>
+    <t>semi-supervised, laplacian eigenmaps</t>
+  </si>
+  <si>
+    <t>extensive discussion of semi-supervised manifold learning, details on laplacian</t>
+  </si>
+  <si>
+    <t>bengio, paiement, vincent, delalleau, le roux, ouimet</t>
+  </si>
+  <si>
+    <t>out-of-sample extensions for lle, isomap, mds, eigenmaps, and spectral clustering</t>
+  </si>
+  <si>
+    <t>generalization</t>
+  </si>
+  <si>
+    <t>for outlook, discussion</t>
+  </si>
+  <si>
+    <t>goldberg, zakai, kushnir, ritov</t>
+  </si>
+  <si>
+    <t>manifold learning: the price of normalization</t>
+  </si>
+  <si>
+    <t>he, cai, yan, zhang</t>
+  </si>
+  <si>
+    <t>neighborhood-preserving-embedding</t>
+  </si>
+  <si>
+    <t>discussion, alternative</t>
+  </si>
+  <si>
+    <t>kokiopoulou, saad</t>
+  </si>
+  <si>
+    <t>orthogonal neighborhood preserving projections: a projection-based dimensionality reduction technique</t>
+  </si>
+  <si>
+    <t>salakhutdinov, hinton</t>
+  </si>
+  <si>
+    <t>learning a nonlinear embedding by preserving class neighbourhood structure</t>
+  </si>
+  <si>
+    <t>sha, saul</t>
+  </si>
+  <si>
+    <t>analysis and extension of spectral methods for nonlinear dimensionality reduction</t>
+  </si>
+  <si>
+    <t>neighborhood-preserving</t>
+  </si>
+  <si>
+    <t>angle-preserving</t>
+  </si>
+  <si>
+    <t>extension maximally preserving angles, perhaps include in experiments</t>
+  </si>
+  <si>
+    <t>saul, weinberger, sha, ham, lee</t>
+  </si>
+  <si>
+    <t>spectral methods for dimensionality reduction</t>
+  </si>
+  <si>
+    <t>overview on spectral methods</t>
+  </si>
+  <si>
+    <t>chen, wang, li, sun</t>
+  </si>
+  <si>
+    <t>robust semi-supervised manifold learning algorithm for classification</t>
+  </si>
+  <si>
+    <t>robust, noisy data</t>
+  </si>
+  <si>
+    <t>symons</t>
+  </si>
+  <si>
+    <t>error-bounded graph construction for semi-supervised manifold learning</t>
+  </si>
+  <si>
+    <t>reconstruction error, neighborhood</t>
   </si>
 </sst>
 </file>
@@ -138,8 +291,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,122 +611,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="64.08984375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1985</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B5" s="1">
+        <v>2001</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2002</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2002</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
         <v>2003</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2004</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B14" s="1">
         <v>2006</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>2000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>2003</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2007</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2008</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2009</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
+      <sortCondition ref="B1:B8"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F6">
+    <sortCondition ref="B1:B6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started to write intro
</commit_message>
<xml_diff>
--- a/1_literature/literature-list.xlsx
+++ b/1_literature/literature-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42535091-B349-4DFF-B35F-6193E52D8908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18586325-7D88-4733-B07A-786F23A1CB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
   <si>
     <t>authors</t>
   </si>
@@ -256,6 +256,24 @@
   </si>
   <si>
     <t>reconstruction error, neighborhood</t>
+  </si>
+  <si>
+    <t>cayton</t>
+  </si>
+  <si>
+    <t>algorithms for manifold learning</t>
+  </si>
+  <si>
+    <t>verleysen, francois</t>
+  </si>
+  <si>
+    <t>the curse of dimensionality in data mining and time series prediction</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>intro</t>
   </si>
 </sst>
 </file>
@@ -611,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,6 +1066,46 @@
         <v>49</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">

</xml_diff>

<commit_message>
finished first draft of introduction
</commit_message>
<xml_diff>
--- a/1_literature/literature-list.xlsx
+++ b/1_literature/literature-list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18586325-7D88-4733-B07A-786F23A1CB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42D4FC8-DA00-4903-82B3-845BD45FEB90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>authors</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>intro</t>
+  </si>
+  <si>
+    <t>leist, playne, hawick</t>
+  </si>
+  <si>
+    <t>exploiting graphical processing units for data-parallel scientific applications</t>
+  </si>
+  <si>
+    <t>gpu</t>
+  </si>
+  <si>
+    <t>doshi-velez, kim</t>
+  </si>
+  <si>
+    <t>towards a rigorous science of interpretable machine learning</t>
+  </si>
+  <si>
+    <t>interpretable machine learning</t>
   </si>
 </sst>
 </file>
@@ -629,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1106,6 +1124,46 @@
         <v>78</v>
       </c>
     </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2009</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">

</xml_diff>

<commit_message>
worked on math intro chapter
</commit_message>
<xml_diff>
--- a/1_literature/literature-list.xlsx
+++ b/1_literature/literature-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE852F-B31A-4FBA-A93D-0FE9C59F7985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00ED226-1F4E-4994-9802-705003D228D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
   <si>
     <t>authors</t>
   </si>
@@ -304,6 +304,54 @@
   </si>
   <si>
     <t>perhaps use?</t>
+  </si>
+  <si>
+    <t>mukherjee</t>
+  </si>
+  <si>
+    <t>differential topology</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>topology</t>
+  </si>
+  <si>
+    <t>basic math</t>
+  </si>
+  <si>
+    <t>waldmann</t>
+  </si>
+  <si>
+    <t>topology - an introduction</t>
+  </si>
+  <si>
+    <t>weintraub</t>
+  </si>
+  <si>
+    <t>fundamentals of algebraic topology</t>
+  </si>
+  <si>
+    <t>choquet</t>
+  </si>
+  <si>
+    <t>hurtado, markvorsen, min-oo, palmer</t>
+  </si>
+  <si>
+    <t>global riemannian geometry: curvature and topology</t>
+  </si>
+  <si>
+    <t>ibadula, veys</t>
+  </si>
+  <si>
+    <t>bridging algebra, geometry and topology</t>
+  </si>
+  <si>
+    <t>mccleary</t>
+  </si>
+  <si>
+    <t>a first course in topology</t>
   </si>
 </sst>
 </file>
@@ -659,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,373 +746,373 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1">
-        <v>1985</v>
+        <v>1966</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
-        <v>2000</v>
+        <v>1985</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>2000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
         <v>2002</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>2003</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>46</v>
+      <c r="A10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>2003</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2004</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1">
         <v>2005</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
         <v>2005</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1">
         <v>2005</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>2006</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1">
         <v>2006</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B20" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
@@ -1078,79 +1126,79 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1">
         <v>2008</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>2009</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1">
-        <v>2017</v>
+        <v>2009</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>78</v>
@@ -1158,47 +1206,187 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B25" s="1">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B31" s="1">
         <v>2018</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F26">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
       <sortCondition ref="B1:B8"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
adapted intro to ext abstr
</commit_message>
<xml_diff>
--- a/1_literature/literature-list.xlsx
+++ b/1_literature/literature-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00ED226-1F4E-4994-9802-705003D228D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0CD88C-8EBF-40E0-8C25-F2E8CB3F5174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>h-lle</t>
   </si>
   <si>
-    <t>original proposition of h-lle, contrast to laplacian and lle</t>
-  </si>
-  <si>
     <t>tenenbaum, de silva, langford</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>a first course in topology</t>
+  </si>
+  <si>
+    <t>original proposition of h-lle, contrast to laplacian and lle, plus link to code</t>
   </si>
 </sst>
 </file>
@@ -709,15 +709,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" style="2" customWidth="1"/>
     <col min="2" max="2" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="5.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="64.08984375" style="2" customWidth="1"/>
@@ -746,42 +746,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1">
         <v>1966</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>1985</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -806,22 +806,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>2000</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -832,7 +832,7 @@
         <v>2001</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>
@@ -841,47 +841,47 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>2002</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1">
         <v>2002</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -921,27 +921,27 @@
         <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1">
         <v>2003</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -952,96 +952,96 @@
         <v>2004</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1">
         <v>2005</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1">
         <v>2005</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1">
         <v>2005</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1">
         <v>2005</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1066,322 +1066,322 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1">
         <v>2006</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1">
         <v>2006</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1">
         <v>2007</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1">
         <v>2008</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1">
         <v>2008</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>2009</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1">
         <v>2009</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1">
         <v>2014</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1">
         <v>2014</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="1">
         <v>2014</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1">
         <v>2015</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1">
         <v>2017</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1">
         <v>2018</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1">
         <v>2018</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B32" s="1">
         <v>2020</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="1">
         <v>2006</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>